<commit_message>
6. Rest of new Home Page items  + track button
</commit_message>
<xml_diff>
--- a/DataSource/Olyve.xlsx
+++ b/DataSource/Olyve.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mokingjay_Olyve\DataSource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Syoussef\PycharmProjects\Mokingjay_Olyve\DataSource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11010" windowHeight="4215" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11010" windowHeight="4215"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="113">
   <si>
     <t>Product Name</t>
   </si>
@@ -299,18 +299,12 @@
     <t>Home</t>
   </si>
   <si>
-    <t>Number 39</t>
-  </si>
-  <si>
     <t>https://olyve.olyveinc.com/viewer</t>
   </si>
   <si>
     <t>Gift View</t>
   </si>
   <si>
-    <t>0020102515</t>
-  </si>
-  <si>
     <t>Delivery Day</t>
   </si>
   <si>
@@ -320,37 +314,58 @@
     <t>Bird Road, Miami, FL, United States Billing</t>
   </si>
   <si>
-    <t>Number 39 Billing</t>
-  </si>
-  <si>
     <t>D:\Mokingjay_Olyve\DataSource\mockingjay.png</t>
   </si>
   <si>
     <t>D:\Mokingjay_Olyve\DataSource\SampleVideo_1280x720_1mb.mp4</t>
   </si>
   <si>
-    <t>kmohamed@integrant.com</t>
-  </si>
-  <si>
     <t>0020102516</t>
   </si>
   <si>
-    <t>Number 40</t>
-  </si>
-  <si>
-    <t>Happy</t>
-  </si>
-  <si>
-    <t>Number 40 Billing</t>
-  </si>
-  <si>
-    <t>Business</t>
-  </si>
-  <si>
-    <t>I am Happy</t>
-  </si>
-  <si>
-    <t>Anastasia Avenue, Coral Gables, FL, United States</t>
+    <t>shagagi@integrant.com</t>
+  </si>
+  <si>
+    <t>The Olyve Experience</t>
+  </si>
+  <si>
+    <t>https://olyve.olyveinc.com/c/theolyveexperience/</t>
+  </si>
+  <si>
+    <t>https://olyve.olyveinc.com/c/olyvecustomers/</t>
+  </si>
+  <si>
+    <t>From Our Customer</t>
+  </si>
+  <si>
+    <t>https://olyve.olyveinc.com/track</t>
+  </si>
+  <si>
+    <t>Track</t>
+  </si>
+  <si>
+    <t>Order ID</t>
+  </si>
+  <si>
+    <t>https://olyve.olyveinc.com/c/sipsandstems/</t>
+  </si>
+  <si>
+    <t>WorkShop</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>https://olyve.olyveinc.com/service</t>
+  </si>
+  <si>
+    <t>PIN Code</t>
+  </si>
+  <si>
+    <t>Number 50</t>
+  </si>
+  <si>
+    <t>Number 50 Billing</t>
   </si>
 </sst>
 </file>
@@ -395,7 +410,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -417,6 +432,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -698,14 +714,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -810,6 +826,62 @@
       </c>
       <c r="B13" s="3" t="s">
         <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B17">
+        <v>14061217</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19">
+        <v>124500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -821,6 +893,11 @@
     <hyperlink ref="B11" r:id="rId5"/>
     <hyperlink ref="B12" r:id="rId6"/>
     <hyperlink ref="B13" r:id="rId7"/>
+    <hyperlink ref="B14" r:id="rId8"/>
+    <hyperlink ref="B15" r:id="rId9"/>
+    <hyperlink ref="B16" r:id="rId10"/>
+    <hyperlink ref="B20" r:id="rId11"/>
+    <hyperlink ref="B18" r:id="rId12"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -921,14 +998,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
@@ -1010,7 +1085,7 @@
         <v>61</v>
       </c>
       <c r="Q1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="R1" t="s">
         <v>64</v>
@@ -1075,10 +1150,10 @@
         <v>42</v>
       </c>
       <c r="G2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="I2" t="s">
         <v>59</v>
@@ -1086,11 +1161,11 @@
       <c r="J2" t="s">
         <v>56</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="11">
         <v>5.25</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="M2" t="s">
         <v>39</v>
@@ -1099,13 +1174,13 @@
         <v>89</v>
       </c>
       <c r="O2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="P2" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
       <c r="Q2" s="9">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>86</v>
@@ -1114,16 +1189,16 @@
         <v>33122</v>
       </c>
       <c r="T2" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="U2" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="W2" s="8" t="s">
         <v>97</v>
-      </c>
-      <c r="V2" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="W2" s="8" t="s">
-        <v>93</v>
       </c>
       <c r="X2" s="5" t="s">
         <v>39</v>
@@ -1148,106 +1223,28 @@
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3" s="5">
-        <v>33129</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="G3" t="s">
-        <v>98</v>
-      </c>
-      <c r="H3" t="s">
-        <v>99</v>
-      </c>
-      <c r="I3" t="s">
-        <v>59</v>
-      </c>
-      <c r="J3" t="s">
-        <v>56</v>
-      </c>
-      <c r="K3">
-        <v>6.65</v>
-      </c>
-      <c r="L3" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="M3" t="s">
-        <v>39</v>
-      </c>
-      <c r="N3" t="s">
-        <v>105</v>
-      </c>
-      <c r="O3" t="s">
-        <v>95</v>
-      </c>
-      <c r="P3" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q3" s="9">
-        <v>15</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="S3" s="5">
-        <v>33129</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="V3" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="W3" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="X3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z3" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA3" s="5">
-        <v>10</v>
-      </c>
-      <c r="AB3" s="5">
-        <v>20</v>
-      </c>
-      <c r="AC3" s="5">
-        <v>110</v>
-      </c>
-      <c r="AD3" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>81</v>
-      </c>
+      <c r="Y3" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N3">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N1048576">
       <formula1>"Home, Business, Hospital, Dormitory"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X1:X1048576 D1:D1048576 AE1:AE1048576">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y1:Y1048576">
+      <formula1>"Bonkers!, nope, beauty 10"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M1048576">
+      <formula1>"Yes"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="V2" r:id="rId1"/>
-    <hyperlink ref="V3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1255,7 +1252,7 @@
           <x14:formula1>
             <xm:f>Products!$A$2:$A$8</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A3</xm:sqref>
+          <xm:sqref>A1:A1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1317,10 +1314,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sarah & Kholoud 1. Fix Deliverydate. 2. Fix Photo or Video upload. 3. Update Olyve promo codes
</commit_message>
<xml_diff>
--- a/DataSource/Olyve.xlsx
+++ b/DataSource/Olyve.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Syoussef\PycharmProjects\Mokingjay_Olyve\DataSource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mokingjay_Olyve\DataSource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11010" windowHeight="4215"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="118">
   <si>
     <t>Product Name</t>
   </si>
@@ -314,12 +314,6 @@
     <t>Bird Road, Miami, FL, United States Billing</t>
   </si>
   <si>
-    <t>D:\Mokingjay_Olyve\DataSource\mockingjay.png</t>
-  </si>
-  <si>
-    <t>D:\Mokingjay_Olyve\DataSource\SampleVideo_1280x720_1mb.mp4</t>
-  </si>
-  <si>
     <t>0020102516</t>
   </si>
   <si>
@@ -362,10 +356,31 @@
     <t>PIN Code</t>
   </si>
   <si>
+    <t>nope</t>
+  </si>
+  <si>
     <t>Number 50</t>
   </si>
   <si>
     <t>Number 50 Billing</t>
+  </si>
+  <si>
+    <t>Promotion Code Text</t>
+  </si>
+  <si>
+    <t>Premiere discount was applied!</t>
+  </si>
+  <si>
+    <t>Discount Text</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>DataSource\mockingjay.png</t>
+  </si>
+  <si>
+    <t>DataSource\SampleVideo_1280x720_1mb.mp4</t>
   </si>
 </sst>
 </file>
@@ -432,7 +447,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -716,7 +731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -830,31 +845,31 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B17">
         <v>14061217</v>
@@ -862,15 +877,15 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B19">
         <v>124500</v>
@@ -878,10 +893,10 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -996,9 +1011,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1033,9 +1050,11 @@
     <col min="29" max="29" width="15" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="16" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1129,8 +1148,14 @@
       <c r="AE1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1150,10 +1175,10 @@
         <v>42</v>
       </c>
       <c r="G2" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="H2" t="s">
-        <v>96</v>
+        <v>117</v>
       </c>
       <c r="I2" t="s">
         <v>59</v>
@@ -1162,10 +1187,10 @@
         <v>56</v>
       </c>
       <c r="K2" s="11">
-        <v>5.25</v>
+        <v>0.1</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M2" t="s">
         <v>39</v>
@@ -1177,7 +1202,7 @@
         <v>93</v>
       </c>
       <c r="P2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Q2" s="9">
         <v>22</v>
@@ -1192,17 +1217,20 @@
         <v>94</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="W2" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="X2" s="5" t="s">
         <v>39</v>
       </c>
+      <c r="Y2" s="5" t="s">
+        <v>109</v>
+      </c>
       <c r="Z2" s="8" t="s">
         <v>74</v>
       </c>
@@ -1221,8 +1249,14 @@
       <c r="AE2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AF2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="Y3" s="5"/>
     </row>
   </sheetData>
@@ -1234,17 +1268,14 @@
       <formula1>"Yes, No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y1:Y1048576">
-      <formula1>"Bonkers!, nope, beauty 10"</formula1>
+      <formula1>"Bonkers!, nope, beauty10"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M1048576">
       <formula1>"Yes"</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">

</xml_diff>

<commit_message>
Trial in Olyve Promotion Code
</commit_message>
<xml_diff>
--- a/DataSource/Olyve.xlsx
+++ b/DataSource/Olyve.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mokingjay_Olyve\DataSource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Syoussef\PycharmProjects\Mokingjay_Olyve\DataSource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -356,9 +356,6 @@
     <t>PIN Code</t>
   </si>
   <si>
-    <t>nope</t>
-  </si>
-  <si>
     <t>Number 50</t>
   </si>
   <si>
@@ -381,6 +378,9 @@
   </si>
   <si>
     <t>DataSource\SampleVideo_1280x720_1mb.mp4</t>
+  </si>
+  <si>
+    <t>beauty10</t>
   </si>
 </sst>
 </file>
@@ -1013,9 +1013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1149,10 +1147,10 @@
         <v>80</v>
       </c>
       <c r="AF1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AG1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
@@ -1175,10 +1173,10 @@
         <v>42</v>
       </c>
       <c r="G2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H2" t="s">
         <v>116</v>
-      </c>
-      <c r="H2" t="s">
-        <v>117</v>
       </c>
       <c r="I2" t="s">
         <v>59</v>
@@ -1187,7 +1185,7 @@
         <v>56</v>
       </c>
       <c r="K2" s="11">
-        <v>0.1</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="L2" s="8" t="s">
         <v>95</v>
@@ -1202,10 +1200,10 @@
         <v>93</v>
       </c>
       <c r="P2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q2" s="9">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>86</v>
@@ -1217,7 +1215,7 @@
         <v>94</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="V2" s="7" t="s">
         <v>96</v>
@@ -1229,7 +1227,7 @@
         <v>39</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="Z2" s="8" t="s">
         <v>74</v>
@@ -1250,10 +1248,10 @@
         <v>81</v>
       </c>
       <c r="AF2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AG2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Excel sheet timing issue + Olyve Premier Code Run issue partially solved
</commit_message>
<xml_diff>
--- a/DataSource/Olyve.xlsx
+++ b/DataSource/Olyve.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11010" windowHeight="4215"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="2" r:id="rId1"/>
@@ -365,22 +365,22 @@
     <t>Promotion Code Text</t>
   </si>
   <si>
+    <t>Discount Text</t>
+  </si>
+  <si>
     <t>Premiere discount was applied!</t>
   </si>
   <si>
-    <t>Discount Text</t>
-  </si>
-  <si>
     <t>Discount</t>
   </si>
   <si>
+    <t>Bonkers!</t>
+  </si>
+  <si>
     <t>DataSource\mockingjay.png</t>
   </si>
   <si>
     <t>DataSource\SampleVideo_1280x720_1mb.mp4</t>
-  </si>
-  <si>
-    <t>Bonkers!</t>
   </si>
 </sst>
 </file>
@@ -425,7 +425,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
@@ -448,6 +448,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -731,7 +732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1011,9 +1012,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG3"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1023,21 +1024,21 @@
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="62.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="43" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="59.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="41.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="48" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="15.85546875" bestFit="1" customWidth="1"/>
@@ -1049,7 +1050,7 @@
     <col min="30" max="30" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="16" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.25">
@@ -1150,7 +1151,7 @@
         <v>111</v>
       </c>
       <c r="AG1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
@@ -1173,10 +1174,10 @@
         <v>42</v>
       </c>
       <c r="G2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I2" t="s">
         <v>59</v>
@@ -1203,7 +1204,7 @@
         <v>109</v>
       </c>
       <c r="Q2" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>86</v>
@@ -1227,7 +1228,7 @@
         <v>39</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="Z2" s="8" t="s">
         <v>74</v>
@@ -1247,41 +1248,41 @@
       <c r="AE2" t="s">
         <v>81</v>
       </c>
-      <c r="AF2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG2" t="s">
+      <c r="AF2" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="AG2" s="12" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="Y3" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N2">
       <formula1>"Home, Business, Hospital, Dormitory"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X1:X1048576 D1:D1048576 AE1:AE1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE1:AE2 D1:D2 X1:X2">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y1:Y1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y1:Y2">
       <formula1>"Bonkers!, nope, beauty10"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M2">
       <formula1>"Yes"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="V2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Products!$A$2:$A$8</xm:f>
+            <xm:f>Products!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>A1:A1048576</xm:sqref>
+          <xm:sqref>A1:A2</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Resolving Product Name check Adding Negavtive Scenarios (not working)
</commit_message>
<xml_diff>
--- a/DataSource/Olyve.xlsx
+++ b/DataSource/Olyve.xlsx
@@ -9,14 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11010" windowHeight="4215"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11010" windowHeight="4215" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="2" r:id="rId1"/>
     <sheet name="Products" sheetId="1" r:id="rId2"/>
     <sheet name="OrderInfo" sheetId="3" r:id="rId3"/>
     <sheet name="GeneralInfo" sheetId="4" r:id="rId4"/>
+    <sheet name="Negative" sheetId="5" r:id="rId5"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="137">
   <si>
     <t>Product Name</t>
   </si>
@@ -374,13 +378,70 @@
     <t>Discount</t>
   </si>
   <si>
-    <t>Bonkers!</t>
-  </si>
-  <si>
     <t>DataSource\mockingjay.png</t>
   </si>
   <si>
     <t>DataSource\SampleVideo_1280x720_1mb.mp4</t>
+  </si>
+  <si>
+    <t>Product CheckOut Name</t>
+  </si>
+  <si>
+    <t>OLYVE + JAMES</t>
+  </si>
+  <si>
+    <t>beauty10</t>
+  </si>
+  <si>
+    <t>Invalid Zip Code</t>
+  </si>
+  <si>
+    <t>Invalid Zip Code Characters</t>
+  </si>
+  <si>
+    <t>ABCDE</t>
+  </si>
+  <si>
+    <t>Invalid Name</t>
+  </si>
+  <si>
+    <t>#*$*#)@)@</t>
+  </si>
+  <si>
+    <t>Error Missing Name Zip Code</t>
+  </si>
+  <si>
+    <t>Error Invalid Zip Code</t>
+  </si>
+  <si>
+    <t>Error Invalid Name</t>
+  </si>
+  <si>
+    <t>Hi. please enter a valid zip code.</t>
+  </si>
+  <si>
+    <t>This field is required</t>
+  </si>
+  <si>
+    <t>Valid Name</t>
+  </si>
+  <si>
+    <t>Valid Zip Code</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Error Zip Code Unsupported Header</t>
+  </si>
+  <si>
+    <t>Error Zip Code Unsupported Body</t>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
+  <si>
+    <t>Oops! There is a problem. Please enter a valid zip code. Reference: b0ba9c0add33</t>
   </si>
 </sst>
 </file>
@@ -465,6 +526,25 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Home"/>
+      <sheetName val="Products"/>
+      <sheetName val="OrderInfo"/>
+      <sheetName val="GeneralInfo"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -732,7 +812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1012,266 +1092,278 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="43" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="59.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="41.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="48" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="AB1" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC1" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AF1" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AG1" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="AF1" t="s">
-        <v>111</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:34" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="5">
+      <c r="D2" s="5">
         <v>33122</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="H2" t="s">
-        <v>117</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="11">
+      <c r="L2" s="11">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="M2" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="Q2" s="9">
+      <c r="R2" s="9">
         <v>22</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="S2" s="5">
+      <c r="T2" s="5">
         <v>33122</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="U2" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="V2" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="W2" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="X2" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="Y2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Y2" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="Z2" s="8" t="s">
+      <c r="Z2" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="AA2" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="AB2" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC2" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="AA2" s="5">
+      <c r="AD2" s="5">
         <v>10</v>
       </c>
-      <c r="AB2" s="5">
+      <c r="AE2" s="5">
         <v>20</v>
       </c>
-      <c r="AC2" s="5">
+      <c r="AF2" s="5">
         <v>110</v>
       </c>
-      <c r="AD2" s="10" t="s">
+      <c r="AG2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AH2" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="AF2" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="AG2" s="12" t="s">
-        <v>114</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N2">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O1:O2">
       <formula1>"Home, Business, Hospital, Dormitory"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE1:AE2 D1:D2 X1:X2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH1:AH2 E1:E2 Y1:Y2">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y1:Y2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z1:Z2">
       <formula1>"Bonkers!, nope, beauty10"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N2">
       <formula1>"Yes"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"OLYVE + ELLIOT,OLYVE + JAMES,OLYVE + LIAM,OLYVE + OLIVIA,OLYVE + TASHA,OLYVE + LUCY,OLYVE + GWEN"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1"/>
+    <hyperlink ref="W2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1280,7 +1372,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Products!#REF!</xm:f>
+            <xm:f>[1]Products!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>A1:A2</xm:sqref>
         </x14:dataValidation>
@@ -1360,4 +1452,109 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="74.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1" t="s">
+        <v>133</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2">
+        <v>33122</v>
+      </c>
+      <c r="D2">
+        <v>99387</v>
+      </c>
+      <c r="E2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H2" t="s">
+        <v>128</v>
+      </c>
+      <c r="J2" t="s">
+        <v>135</v>
+      </c>
+      <c r="K2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]Products!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>A1:A2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Handling the products that don't have accessory page and fixing all the related locators
</commit_message>
<xml_diff>
--- a/DataSource/Olyve.xlsx
+++ b/DataSource/Olyve.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Syoussef\PycharmProjects\Mokingjay_Olyve\DataSource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mokingjay_Olyve\DataSource\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11010" windowHeight="4215"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11010" windowHeight="4215" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="126">
   <si>
     <t>Product Name</t>
   </si>
@@ -317,70 +317,94 @@
     <t>0020102516</t>
   </si>
   <si>
+    <t>The Olyve Experience</t>
+  </si>
+  <si>
+    <t>https://olyve.olyveinc.com/c/theolyveexperience/</t>
+  </si>
+  <si>
+    <t>https://olyve.olyveinc.com/c/olyvecustomers/</t>
+  </si>
+  <si>
+    <t>From Our Customer</t>
+  </si>
+  <si>
+    <t>https://olyve.olyveinc.com/track</t>
+  </si>
+  <si>
+    <t>Track</t>
+  </si>
+  <si>
+    <t>Order ID</t>
+  </si>
+  <si>
+    <t>https://olyve.olyveinc.com/c/sipsandstems/</t>
+  </si>
+  <si>
+    <t>WorkShop</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>https://olyve.olyveinc.com/service</t>
+  </si>
+  <si>
+    <t>PIN Code</t>
+  </si>
+  <si>
+    <t>Number 50</t>
+  </si>
+  <si>
+    <t>Number 50 Billing</t>
+  </si>
+  <si>
+    <t>Promotion Code Text</t>
+  </si>
+  <si>
+    <t>Discount Text</t>
+  </si>
+  <si>
+    <t>Premiere discount was applied!</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>Bonkers!</t>
+  </si>
+  <si>
+    <t>DataSource\mockingjay.png</t>
+  </si>
+  <si>
+    <t>DataSource\SampleVideo_1280x720_1mb.mp4</t>
+  </si>
+  <si>
+    <t>kmohamed@integrant.com</t>
+  </si>
+  <si>
+    <t>Business</t>
+  </si>
+  <si>
+    <t>Number 60 Billing</t>
+  </si>
+  <si>
+    <t>0020102517</t>
+  </si>
+  <si>
+    <t>Number 51</t>
+  </si>
+  <si>
+    <t>Test Gift Message</t>
+  </si>
+  <si>
+    <t>Happy</t>
+  </si>
+  <si>
+    <t>I am Happy</t>
+  </si>
+  <si>
     <t>shagagi@integrant.com</t>
-  </si>
-  <si>
-    <t>The Olyve Experience</t>
-  </si>
-  <si>
-    <t>https://olyve.olyveinc.com/c/theolyveexperience/</t>
-  </si>
-  <si>
-    <t>https://olyve.olyveinc.com/c/olyvecustomers/</t>
-  </si>
-  <si>
-    <t>From Our Customer</t>
-  </si>
-  <si>
-    <t>https://olyve.olyveinc.com/track</t>
-  </si>
-  <si>
-    <t>Track</t>
-  </si>
-  <si>
-    <t>Order ID</t>
-  </si>
-  <si>
-    <t>https://olyve.olyveinc.com/c/sipsandstems/</t>
-  </si>
-  <si>
-    <t>WorkShop</t>
-  </si>
-  <si>
-    <t>Service</t>
-  </si>
-  <si>
-    <t>https://olyve.olyveinc.com/service</t>
-  </si>
-  <si>
-    <t>PIN Code</t>
-  </si>
-  <si>
-    <t>Number 50</t>
-  </si>
-  <si>
-    <t>Number 50 Billing</t>
-  </si>
-  <si>
-    <t>Promotion Code Text</t>
-  </si>
-  <si>
-    <t>Discount Text</t>
-  </si>
-  <si>
-    <t>Premiere discount was applied!</t>
-  </si>
-  <si>
-    <t>Discount</t>
-  </si>
-  <si>
-    <t>Bonkers!</t>
-  </si>
-  <si>
-    <t>DataSource\mockingjay.png</t>
-  </si>
-  <si>
-    <t>DataSource\SampleVideo_1280x720_1mb.mp4</t>
   </si>
 </sst>
 </file>
@@ -732,7 +756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -846,31 +870,31 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B17">
         <v>14061217</v>
@@ -878,15 +902,15 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B19">
         <v>124500</v>
@@ -894,10 +918,10 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -923,7 +947,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1012,9 +1038,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1148,10 +1176,10 @@
         <v>80</v>
       </c>
       <c r="AF1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG1" t="s">
         <v>111</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
@@ -1174,10 +1202,10 @@
         <v>42</v>
       </c>
       <c r="G2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H2" t="s">
         <v>116</v>
-      </c>
-      <c r="H2" t="s">
-        <v>117</v>
       </c>
       <c r="I2" t="s">
         <v>59</v>
@@ -1201,10 +1229,10 @@
         <v>93</v>
       </c>
       <c r="P2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q2" s="9">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>86</v>
@@ -1216,10 +1244,10 @@
         <v>94</v>
       </c>
       <c r="U2" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>96</v>
+        <v>125</v>
       </c>
       <c r="W2" s="8" t="s">
         <v>95</v>
@@ -1228,7 +1256,7 @@
         <v>39</v>
       </c>
       <c r="Y2" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Z2" s="8" t="s">
         <v>74</v>
@@ -1249,32 +1277,134 @@
         <v>81</v>
       </c>
       <c r="AF2" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG2" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="AG2" s="12" t="s">
+    </row>
+    <row r="3" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="5">
+        <v>33122</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q3" s="9">
+        <v>29</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="S3" s="5">
+        <v>33122</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="V3" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="W3" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y3" s="5" t="s">
         <v>114</v>
+      </c>
+      <c r="Z3" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA3" s="5">
+        <v>10</v>
+      </c>
+      <c r="AB3" s="5">
+        <v>20</v>
+      </c>
+      <c r="AC3" s="5">
+        <v>110</v>
+      </c>
+      <c r="AD3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE3" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF3" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG3" s="12" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N3">
       <formula1>"Home, Business, Hospital, Dormitory"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE1:AE2 D1:D2 X1:X2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE1:AE3 D1:D3 X1:X3">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y1:Y2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y1:Y3">
       <formula1>"Bonkers!, nope, beauty10"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M3">
       <formula1>"Yes"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1"/>
+    <hyperlink ref="V3" r:id="rId1"/>
+    <hyperlink ref="V2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1282,7 +1412,7 @@
           <x14:formula1>
             <xm:f>Products!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>A1:A2</xm:sqref>
+          <xm:sqref>A1:A3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Add wait for apply promo code button and make sure all promo codes are working for the products that don't have accessories option
</commit_message>
<xml_diff>
--- a/DataSource/Olyve.xlsx
+++ b/DataSource/Olyve.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="137">
   <si>
     <t>Product Name</t>
   </si>
@@ -405,6 +405,39 @@
   </si>
   <si>
     <t>shagagi@integrant.com</t>
+  </si>
+  <si>
+    <t>beauty10</t>
+  </si>
+  <si>
+    <t>Life</t>
+  </si>
+  <si>
+    <t>Life is Beautiful</t>
+  </si>
+  <si>
+    <t>2010121457</t>
+  </si>
+  <si>
+    <t>Hospital</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cape Florida Drive, Miami, FL, United States</t>
+  </si>
+  <si>
+    <t>Number 52</t>
+  </si>
+  <si>
+    <t>Life is Good</t>
+  </si>
+  <si>
+    <t>Number 70 Billing</t>
+  </si>
+  <si>
+    <t>0120124525</t>
+  </si>
+  <si>
+    <t>nope</t>
   </si>
 </sst>
 </file>
@@ -948,7 +981,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,10 +1071,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG3"/>
+  <dimension ref="A1:AG4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,7 +1083,7 @@
     <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="43" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="59.85546875" bestFit="1" customWidth="1"/>
@@ -1232,7 +1265,7 @@
         <v>108</v>
       </c>
       <c r="Q2" s="9">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>86</v>
@@ -1333,7 +1366,7 @@
         <v>121</v>
       </c>
       <c r="Q3" s="9">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="R3" s="5" t="s">
         <v>124</v>
@@ -1357,7 +1390,7 @@
         <v>39</v>
       </c>
       <c r="Y3" s="5" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="Z3" s="8" t="s">
         <v>74</v>
@@ -1384,27 +1417,120 @@
         <v>113</v>
       </c>
     </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="5">
+        <v>33149</v>
+      </c>
+      <c r="E4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F4" t="s">
+        <v>127</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4" s="11">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="O4" t="s">
+        <v>131</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q4" s="9">
+        <v>20</v>
+      </c>
+      <c r="R4" t="s">
+        <v>133</v>
+      </c>
+      <c r="S4" s="5">
+        <v>33149</v>
+      </c>
+      <c r="T4" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="V4" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="W4" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="X4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y4" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z4" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA4" s="5">
+        <v>10</v>
+      </c>
+      <c r="AB4" s="5">
+        <v>20</v>
+      </c>
+      <c r="AC4" s="5">
+        <v>110</v>
+      </c>
+      <c r="AD4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE4" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF4" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG4" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N4">
       <formula1>"Home, Business, Hospital, Dormitory"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE1:AE3 D1:D3 X1:X3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE1:AE4 D1:D3 X1:X4">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y1:Y3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y1:Y4">
       <formula1>"Bonkers!, nope, beauty10"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M4">
       <formula1>"Yes"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="V3" r:id="rId1"/>
     <hyperlink ref="V2" r:id="rId2"/>
+    <hyperlink ref="V4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -1412,7 +1538,7 @@
           <x14:formula1>
             <xm:f>Products!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>A1:A3</xm:sqref>
+          <xm:sqref>A1:A4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Fixing second negative test case + adding others tab in configuration file for the negative cases
</commit_message>
<xml_diff>
--- a/DataSource/Olyve.xlsx
+++ b/DataSource/Olyve.xlsx
@@ -9,14 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11010" windowHeight="4215" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11010" windowHeight="4215" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="2" r:id="rId1"/>
     <sheet name="Products" sheetId="1" r:id="rId2"/>
     <sheet name="OrderInfo" sheetId="3" r:id="rId3"/>
     <sheet name="GeneralInfo" sheetId="4" r:id="rId4"/>
+    <sheet name="Others" sheetId="5" r:id="rId5"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId6"/>
+  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="154">
   <si>
     <t>Product Name</t>
   </si>
@@ -438,6 +442,57 @@
   </si>
   <si>
     <t>nope</t>
+  </si>
+  <si>
+    <t>This field is required</t>
+  </si>
+  <si>
+    <t>Valid Name</t>
+  </si>
+  <si>
+    <t>Valid Zip Code</t>
+  </si>
+  <si>
+    <t>Invalid Zip Code</t>
+  </si>
+  <si>
+    <t>Invalid Zip Code Characters</t>
+  </si>
+  <si>
+    <t>Invalid Name</t>
+  </si>
+  <si>
+    <t>Error Missing Name Zip Code</t>
+  </si>
+  <si>
+    <t>Error Invalid Zip Code</t>
+  </si>
+  <si>
+    <t>Error Invalid Name</t>
+  </si>
+  <si>
+    <t>Error Zip Code Unsupported Header</t>
+  </si>
+  <si>
+    <t>Error Zip Code Unsupported Body</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>ABCDE</t>
+  </si>
+  <si>
+    <t>#*$*#)@)@</t>
+  </si>
+  <si>
+    <t>Hi. please enter a valid zip code.</t>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
+  <si>
+    <t>Oops! There is a problem. Please enter a valid zip code. Reference: b0ba9c0add33</t>
   </si>
 </sst>
 </file>
@@ -522,6 +577,25 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Home"/>
+      <sheetName val="Products"/>
+      <sheetName val="OrderInfo"/>
+      <sheetName val="GeneralInfo"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -981,7 +1055,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,7 +1147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
@@ -1616,4 +1690,112 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="74.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="12">
+        <v>33122</v>
+      </c>
+      <c r="D2" s="12">
+        <v>99387</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>[1]Products!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>A1:A2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
All negative cases are passed now except for test invalid name because the errror message text is not exist in the HTML
</commit_message>
<xml_diff>
--- a/DataSource/Olyve.xlsx
+++ b/DataSource/Olyve.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="155">
   <si>
     <t>Product Name</t>
   </si>
@@ -456,9 +456,6 @@
     <t>Invalid Zip Code</t>
   </si>
   <si>
-    <t>Invalid Zip Code Characters</t>
-  </si>
-  <si>
     <t>Invalid Name</t>
   </si>
   <si>
@@ -492,7 +489,13 @@
     <t>ERROR</t>
   </si>
   <si>
-    <t>Oops! There is a problem. Please enter a valid zip code. Reference: b0ba9c0add33</t>
+    <t>Please match the requested format</t>
+  </si>
+  <si>
+    <t>Unsupported Zip Code</t>
+  </si>
+  <si>
+    <t>Oops! There is a problem. Please enter a valid zip code. Reference:</t>
   </si>
 </sst>
 </file>
@@ -1696,8 +1699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1710,7 +1713,7 @@
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="33" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="74.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1729,25 +1732,25 @@
         <v>140</v>
       </c>
       <c r="E1" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>146</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1755,32 +1758,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C2" s="12">
         <v>33122</v>
       </c>
-      <c r="D2" s="12">
-        <v>99387</v>
-      </c>
-      <c r="E2" s="12" t="s">
+      <c r="D2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" s="12">
+        <v>11865</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>149</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>150</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>137</v>
       </c>
       <c r="H2" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="J2" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12" t="s">
-        <v>152</v>
-      </c>
       <c r="K2" s="12" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All negative cases are passed and added to test runner Calculations needs to be revisit because of the products that have a float price
</commit_message>
<xml_diff>
--- a/DataSource/Olyve.xlsx
+++ b/DataSource/Olyve.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11010" windowHeight="4215" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11010" windowHeight="4215" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="2" r:id="rId1"/>
@@ -426,9 +426,6 @@
     <t>Hospital</t>
   </si>
   <si>
-    <t xml:space="preserve"> Cape Florida Drive, Miami, FL, United States</t>
-  </si>
-  <si>
     <t>Number 52</t>
   </si>
   <si>
@@ -489,13 +486,16 @@
     <t>ERROR</t>
   </si>
   <si>
-    <t>Please match the requested format</t>
-  </si>
-  <si>
     <t>Unsupported Zip Code</t>
   </si>
   <si>
     <t>Oops! There is a problem. Please enter a valid zip code. Reference:</t>
+  </si>
+  <si>
+    <t>Hi. We don't allow for numbers or special characters, sorry!</t>
+  </si>
+  <si>
+    <t>Cape Florida Drive, Miami, FL, United States</t>
   </si>
 </sst>
 </file>
@@ -1150,8 +1150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG4"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1529,37 +1529,37 @@
         <v>130</v>
       </c>
       <c r="O4" t="s">
+        <v>154</v>
+      </c>
+      <c r="P4" s="12" t="s">
         <v>131</v>
-      </c>
-      <c r="P4" s="12" t="s">
-        <v>132</v>
       </c>
       <c r="Q4" s="9">
         <v>20</v>
       </c>
       <c r="R4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="S4" s="5">
         <v>33149</v>
       </c>
       <c r="T4" s="12" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="V4" s="7" t="s">
         <v>117</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="X4" s="5" t="s">
         <v>39</v>
       </c>
       <c r="Y4" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="Z4" s="8" t="s">
         <v>74</v>
@@ -1588,16 +1588,16 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3 D1 X1 X2:X4 AE1 AE2:AE4">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1 N2:N4">
       <formula1>"Home, Business, Hospital, Dormitory"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE1:AE4 D1:D3 X1:X4">
-      <formula1>"Yes, No"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y1:Y4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y1 Y2:Y4">
       <formula1>"Bonkers!, nope, beauty10"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1 M2:M4">
       <formula1>"Yes"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1615,7 +1615,7 @@
           <x14:formula1>
             <xm:f>Products!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>A1:A4</xm:sqref>
+          <xm:sqref>A1 A2:A4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1699,8 +1699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1713,7 +1713,7 @@
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="54.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="33" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="74.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1723,34 +1723,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="H1" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="I1" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J1" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="K1" s="12" t="s">
         <v>145</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1758,34 +1758,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C2" s="12">
         <v>33122</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E2" s="12">
         <v>11865</v>
       </c>
       <c r="F2" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="H2" s="12" t="s">
+      <c r="I2" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="J2" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="K2" s="12" t="s">
         <v>152</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Executing the Test Runner from Command Prompt Window + Integration with Jenkins
</commit_message>
<xml_diff>
--- a/DataSource/Olyve.xlsx
+++ b/DataSource/Olyve.xlsx
@@ -594,7 +594,7 @@
     <t>Number 45 Billing</t>
   </si>
   <si>
-    <t>NOW SERVING SOCAL, NYC, PHILLY, + MIAMI</t>
+    <t>GIFT BOX &amp; DELIVERY ALWAYS INCLUDED</t>
   </si>
 </sst>
 </file>
@@ -985,7 +985,7 @@
       <c r="A2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="12" t="s">
         <v>187</v>
       </c>
     </row>

</xml_diff>